<commit_message>
report up to date
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Python Class\Hydraulic Model\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Hydraulic Model V2.0\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="8400" windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>Casing</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Hole Size</t>
+  </si>
+  <si>
+    <t>YPL</t>
   </si>
 </sst>
 </file>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:B56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1415,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="1">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="C14" s="1">
         <v>10000</v>
@@ -1434,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1834,7 +1837,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
report up to date and calculations steps can be input instead of default every 1 foot calculation
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
   <si>
     <t>Casing</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>YPL</t>
+  </si>
+  <si>
+    <t>Calculations step difference</t>
   </si>
 </sst>
 </file>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B61" sqref="A61:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,6 +1151,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1155,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1880,6 +1891,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added more info into the report. Improved motor, mwd and surface pressure drop calculations. Ran against experimental data from grad school and found 86% correlation (probably experimental setup was off calibration).
Ran against water pressure drop in laminar flow data and found 97% correlation.
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8400" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="14400" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
   <si>
     <t>Casing</t>
   </si>
@@ -55,64 +55,67 @@
     <t>Fluid Type (PL/YPL)</t>
   </si>
   <si>
+    <t>Bit Size</t>
+  </si>
+  <si>
+    <t>Flow Rate, gpm</t>
+  </si>
+  <si>
+    <t>Density, ppg</t>
+  </si>
+  <si>
+    <t>Eccentricity</t>
+  </si>
+  <si>
+    <t>Unit System for Output (field or SI)</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>MWD</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Liner</t>
+  </si>
+  <si>
+    <t>Push Pipe</t>
+  </si>
+  <si>
+    <t>Drill Pipe</t>
+  </si>
+  <si>
+    <t>Drill Collar</t>
+  </si>
+  <si>
+    <t>Bit ID</t>
+  </si>
+  <si>
+    <t>Top Depth</t>
+  </si>
+  <si>
+    <t>Bottom Depth</t>
+  </si>
+  <si>
+    <t>Hole Size</t>
+  </si>
+  <si>
+    <t>YPL</t>
+  </si>
+  <si>
+    <t>Calculations step difference</t>
+  </si>
+  <si>
+    <t>Surface lines IADC Class (1,2,3,4)</t>
+  </si>
+  <si>
     <t>PL</t>
-  </si>
-  <si>
-    <t>Bit Size</t>
-  </si>
-  <si>
-    <t>Flow Rate, gpm</t>
-  </si>
-  <si>
-    <t>Density, ppg</t>
-  </si>
-  <si>
-    <t>Eccentricity</t>
-  </si>
-  <si>
-    <t>Unit System for Output (field or SI)</t>
-  </si>
-  <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>MWD</t>
-  </si>
-  <si>
-    <t>Motor</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Liner</t>
-  </si>
-  <si>
-    <t>Push Pipe</t>
-  </si>
-  <si>
-    <t>Drill Pipe</t>
-  </si>
-  <si>
-    <t>Drill Collar</t>
-  </si>
-  <si>
-    <t>Bit ID</t>
-  </si>
-  <si>
-    <t>Top Depth</t>
-  </si>
-  <si>
-    <t>Bottom Depth</t>
-  </si>
-  <si>
-    <t>Hole Size</t>
-  </si>
-  <si>
-    <t>YPL</t>
-  </si>
-  <si>
-    <t>Calculations step difference</t>
   </si>
 </sst>
 </file>
@@ -468,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B61" sqref="A61:B61"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +587,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
@@ -743,10 +746,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -839,8 +842,12 @@
       <c r="B22" s="1">
         <v>6.75</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="C22" s="1">
+        <v>6.75</v>
+      </c>
+      <c r="D22" s="1">
+        <v>6.75</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -854,10 +861,14 @@
         <v>2</v>
       </c>
       <c r="B23" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2.8130000000000002</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -871,10 +882,14 @@
         <v>3</v>
       </c>
       <c r="B24" s="1">
+        <v>10090</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10120</v>
+      </c>
+      <c r="D24" s="1">
         <v>10149</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -890,8 +905,12 @@
       <c r="B25" s="1">
         <v>10000</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1">
+        <v>10090</v>
+      </c>
+      <c r="D25" s="1">
+        <v>10120</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -902,13 +921,17 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -958,7 +981,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1">
         <v>8.5</v>
@@ -966,7 +989,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
         <v>2.7</v>
@@ -974,7 +997,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
         <v>10150</v>
@@ -982,7 +1005,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1">
         <v>10149</v>
@@ -1108,12 +1131,12 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" s="4">
         <v>600</v>
@@ -1121,7 +1144,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="4">
         <v>10</v>
@@ -1129,7 +1152,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="4">
         <v>0</v>
@@ -1137,23 +1160,31 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B56" s="4">
         <v>8.5</v>
       </c>
     </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B61" s="1">
         <v>100</v>
@@ -1168,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:B61"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B24:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,13 +1323,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1410,7 +1441,7 @@
         <v>4.2759999999999998</v>
       </c>
       <c r="C13" s="1">
-        <v>3.8</v>
+        <v>3.8260000000000001</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1461,13 +1492,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1557,13 +1588,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="1">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C22" s="1">
-        <v>4.8</v>
+        <v>5.25</v>
       </c>
       <c r="D22" s="1">
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1578,13 +1609,13 @@
         <v>2</v>
       </c>
       <c r="B23" s="1">
-        <v>3.5</v>
+        <v>2.25</v>
       </c>
       <c r="C23" s="1">
-        <v>2.8</v>
+        <v>2.25</v>
       </c>
       <c r="D23" s="1">
-        <v>2.7</v>
+        <v>2.25</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1638,16 +1669,16 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1698,7 +1729,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1">
         <v>6.75</v>
@@ -1706,7 +1737,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
         <v>2.7</v>
@@ -1714,7 +1745,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
         <v>10150</v>
@@ -1722,7 +1753,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1">
         <v>10149</v>
@@ -1765,13 +1796,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C38" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D38" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E38" s="1">
         <v>13</v>
@@ -1848,20 +1879,20 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" s="4">
-        <v>600</v>
+        <v>300</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="4">
         <v>10</v>
@@ -1869,7 +1900,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B55" s="4">
         <v>0</v>
@@ -1877,23 +1908,31 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B56" s="4">
         <v>6.75</v>
       </c>
     </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B61" s="1">
         <v>100</v>

</xml_diff>

<commit_message>
fixed a bug where and exception was raised if the exact depth of the shoe is not in the list. Error was in report generator while creating the ecd tables. Error was occurring only if calculation steps prevent the exact shoe depth to be in the list. implemented pandas searchsorted and now looking up the nearest depth to the shoe.
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -9,18 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14400" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="18000" windowWidth="28800" windowHeight="12420" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
     <sheet name="well2" sheetId="2" r:id="rId2"/>
+    <sheet name="well3" sheetId="3" r:id="rId3"/>
+    <sheet name="well4" sheetId="4" r:id="rId4"/>
+    <sheet name="well5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="vertical" sheetId="7" r:id="rId7"/>
+    <sheet name="horizontal" sheetId="8" r:id="rId8"/>
+    <sheet name="horizontal_tj" sheetId="9" r:id="rId9"/>
+    <sheet name="vertical_tj" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="32">
   <si>
     <t>Casing</t>
   </si>
@@ -471,7 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -1195,12 +1203,728 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9500</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="M14">
+        <f>10000/30</f>
+        <v>333.33333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9500</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15">
+        <f>M14*1.5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B24:D26"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,6 +2659,4208 @@
         <v>29</v>
       </c>
       <c r="B61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10149</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13:N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9472.4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10149</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9472.4</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.12</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10149</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.875</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15999</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.875</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5.375</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15199</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15999</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="M14">
+        <f>15999/30</f>
+        <v>533.29999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15199</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15">
+        <f>M14*1.5</f>
+        <v>799.94999999999993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="M16">
+        <f>B14-800</f>
+        <v>14399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working version before startinhg to work on tool joint effects implementation
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="18000" windowWidth="28800" windowHeight="12420" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="25200" windowWidth="28800" windowHeight="12420" tabRatio="937" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
@@ -17,18 +17,21 @@
     <sheet name="well3" sheetId="3" r:id="rId3"/>
     <sheet name="well4" sheetId="4" r:id="rId4"/>
     <sheet name="well5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
-    <sheet name="vertical" sheetId="7" r:id="rId7"/>
-    <sheet name="horizontal" sheetId="8" r:id="rId8"/>
-    <sheet name="horizontal_tj" sheetId="9" r:id="rId9"/>
-    <sheet name="vertical_tj" sheetId="10" r:id="rId10"/>
+    <sheet name="vertical" sheetId="7" r:id="rId6"/>
+    <sheet name="horizontal" sheetId="8" r:id="rId7"/>
+    <sheet name="horizontal_tj" sheetId="9" r:id="rId8"/>
+    <sheet name="vertical_tj" sheetId="10" r:id="rId9"/>
+    <sheet name="implement_vertical_tj" sheetId="11" r:id="rId10"/>
+    <sheet name="dswellplan_big_pipe" sheetId="12" r:id="rId11"/>
+    <sheet name="dswellplan_slim_hole" sheetId="13" r:id="rId12"/>
+    <sheet name="dswellplan_big_pipe_tj" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="34">
   <si>
     <t>Casing</t>
   </si>
@@ -124,6 +127,12 @@
   </si>
   <si>
     <t>PL</t>
+  </si>
+  <si>
+    <t>Tool Joint, OD</t>
+  </si>
+  <si>
+    <t>Tool Joint, ID</t>
   </si>
 </sst>
 </file>
@@ -479,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -770,8 +779,12 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.625</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -783,8 +796,12 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.25</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1139,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1205,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1235,7 @@
     <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1287,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1304,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1321,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1321,7 +1338,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1338,7 +1355,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1351,7 +1368,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1364,7 +1381,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1377,7 +1394,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1412,16 +1429,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1">
         <v>5</v>
       </c>
-      <c r="C12" s="1">
-        <v>6.625</v>
-      </c>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1431,16 +1446,14 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="1">
         <v>4.2759999999999998</v>
       </c>
-      <c r="C13" s="1">
-        <v>3.25</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1450,16 +1463,14 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="1">
-        <v>9500</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10000</v>
-      </c>
+        <v>8000</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1468,21 +1479,15 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="M14">
-        <f>10000/30</f>
-        <v>333.33333333333331</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
       </c>
-      <c r="C15" s="1">
-        <v>9500</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1491,21 +1496,15 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="M15">
-        <f>M14*1.5</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1516,8 +1515,12 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.625</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1529,8 +1532,12 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.25</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1724,7 +1731,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="1">
-        <v>10001</v>
+        <v>8001</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1732,7 +1739,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="1">
-        <v>10000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1864,6 +1871,2129 @@
       </c>
       <c r="B53" s="4">
         <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15998</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6.875</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.8260000000000001</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15999</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5.375</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.8130000000000002</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13</v>
+      </c>
+      <c r="F38" s="1">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1">
+        <v>13</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>15198</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15998</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15198</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>15999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1923,8 +4053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4743,21 +6873,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
@@ -5451,11 +7569,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
@@ -6149,7 +8267,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M61"/>
   <sheetViews>
@@ -6867,4 +8985,720 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.625</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <v>8</v>
+      </c>
+      <c r="J11" s="2">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6.625</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.2759999999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>9500</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="M14">
+        <f>10000/30</f>
+        <v>333.33333333333331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9500</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="M15">
+        <f>M14*1.5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2">
+        <v>6</v>
+      </c>
+      <c r="H21" s="2">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>8</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9</v>
+      </c>
+      <c r="K21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>10001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>3</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4</v>
+      </c>
+      <c r="F37" s="3">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3">
+        <v>6</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7</v>
+      </c>
+      <c r="I37" s="3">
+        <v>8</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9</v>
+      </c>
+      <c r="K37" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="1">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
+        <v>16</v>
+      </c>
+      <c r="F38" s="1">
+        <v>16</v>
+      </c>
+      <c r="G38" s="1">
+        <v>16</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>600</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>300</v>
+      </c>
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>200</v>
+      </c>
+      <c r="B48" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>6</v>
+      </c>
+      <c r="B50" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" s="4">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working version. Fixed a bug related to pressure and ecd unit conversion between SI and field units
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="25200" windowWidth="28800" windowHeight="12420" tabRatio="937" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="25800" windowWidth="28800" windowHeight="12420" tabRatio="937"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="36">
   <si>
     <t>Casing</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Tool Joint, ID</t>
+  </si>
+  <si>
+    <t>Tool joint frequency</t>
+  </si>
+  <si>
+    <t>Tool joint length</t>
   </si>
 </sst>
 </file>
@@ -488,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,9 +788,7 @@
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1">
-        <v>6.625</v>
-      </c>
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -799,9 +803,7 @@
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1">
-        <v>3.25</v>
-      </c>
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2632,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="A11:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3327,6 +3329,22 @@
       </c>
       <c r="B61" s="1">
         <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Annulus eccentricity effect is implemented. Working copy before implemeting tool joint effect to inner diameter of drill string.
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="25800" windowWidth="28800" windowHeight="12420" tabRatio="937"/>
+    <workbookView xWindow="0" yWindow="25800" windowWidth="28800" windowHeight="12420" tabRatio="937" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="well1" sheetId="1" r:id="rId1"/>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,9 @@
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>6.625</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -803,7 +805,9 @@
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>3.25</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2636,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="A11:B18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>